<commit_message>
SIR update December 2020
</commit_message>
<xml_diff>
--- a/eT/SIR/downloads/SIR.xlsx
+++ b/eT/SIR/downloads/SIR.xlsx
@@ -33,6 +33,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">β</t>
     </r>
@@ -41,6 +42,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> =</t>
     </r>
@@ -51,6 +53,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">α</t>
     </r>
@@ -59,6 +62,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> =</t>
     </r>
@@ -83,16 +87,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$£-809]#,##0.00;[RED]\-[$£-809]#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,14 +114,14 @@
       <family val="0"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="10"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -138,7 +142,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -162,14 +166,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -180,22 +176,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Result" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1" xfId="23" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -270,10 +262,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0199399924990624"/>
-          <c:y val="0.0199866755496336"/>
-          <c:w val="0.898049756219527"/>
-          <c:h val="0.960026648900733"/>
+          <c:x val="0.0199412389823092"/>
+          <c:y val="0.0199888950583009"/>
+          <c:w val="0.89798087141339"/>
+          <c:h val="0.959911160466408"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -312,6 +304,18 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -638,307 +642,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0.9999</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.996567</c:v>
+                  <c:v>0.9867</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.992580842729667</c:v>
+                  <c:v>0.982764163333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.987821130275849</c:v>
+                  <c:v>0.978077378145773</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.982148578943004</c:v>
+                  <c:v>0.972506855831205</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.975403502996313</c:v>
+                  <c:v>0.9659007755205</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.967404860190204</c:v>
+                  <c:v>0.958087457374567</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.957950240512239</c:v>
+                  <c:v>0.948875410311444</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.946817299848227</c:v>
+                  <c:v>0.93805470550063</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.933767262835291</c:v>
+                  <c:v>0.925400233712916</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.918551218462788</c:v>
+                  <c:v>0.910677490092046</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.900919965024246</c:v>
+                  <c:v>0.893651557064016</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.880638064679464</c:v>
+                  <c:v>0.874099871005258</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.857502462157589</c:v>
+                  <c:v>0.851829093036922</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.831365425483599</c:v>
+                  <c:v>0.826695889684864</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.802160629674685</c:v>
+                  <c:v>0.798630622261778</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.769929964097244</c:v>
+                  <c:v>0.767661872421921</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.734847288085081</c:v>
+                  <c:v>0.733938546657189</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.697234267885565</c:v>
+                  <c:v>0.69774531607299</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.657563141493383</c:v>
+                  <c:v>0.659506809920662</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.61644231646329</c:v>
+                  <c:v>0.619776758280652</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.57458336075644</c:v>
+                  <c:v>0.579210423603692</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.532751854452962</c:v>
+                  <c:v>0.538521953690473</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.491708683256361</c:v>
+                  <c:v>0.498431919994706</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.452151208670608</c:v>
+                  <c:v>0.459613060477541</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.414664122274306</c:v>
+                  <c:v>0.422643014617262</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.379687389210424</c:v>
+                  <c:v>0.387971199760572</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.34750438127287</c:v>
+                  <c:v>0.355903488021004</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.318248701602656</c:v>
+                  <c:v>0.326604280089271</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.291924830671231</c:v>
+                  <c:v>0.300112294957637</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.268436335413865</c:v>
+                  <c:v>0.2763647254536</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.247615832988668</c:v>
+                  <c:v>0.255224405828316</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.229252467620181</c:v>
+                  <c:v>0.236505785302171</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.21311453017179</c:v>
+                  <c:v>0.219997103380249</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.198966449797002</c:v>
+                  <c:v>0.205477658484725</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.186580467144682</c:v>
+                  <c:v>0.192730157160615</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.175743862460282</c:v>
+                  <c:v>0.181548769803166</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.166262788040846</c:v>
+                  <c:v>0.171743782221879</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.157963696006098</c:v>
+                  <c:v>0.163143747896129</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.150693184123072</c:v>
+                  <c:v>0.155595929815883</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.144316886182602</c:v>
+                  <c:v>0.148965656285978</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.138717853033841</c:v>
+                  <c:v>0.143135050927782</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.133794723638358</c:v>
+                  <c:v>0.13800145656536</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.129459875205853</c:v>
+                  <c:v>0.13347576286492</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.125637663304139</c:v>
+                  <c:v>0.129480767138811</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.122262810104594</c:v>
+                  <c:v>0.125949641713959</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.119278964986876</c:v>
+                  <c:v>0.12282454400695</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.116637440989687</c:v>
+                  <c:v>0.120055381785197</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.114296118754061</c:v>
+                  <c:v>0.117598731863795</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.112218503539211</c:v>
+                  <c:v>0.11541690256159</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.110372918427591</c:v>
+                  <c:v>0.113477126376927</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.108731816517381</c:v>
+                  <c:v>0.111750867997076</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.107271195777575</c:v>
+                  <c:v>0.110213232891732</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.105970101713498</c:v>
+                  <c:v>0.108842462688497</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.104810204693302</c:v>
+                  <c:v>0.107619504863773</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.103775440505617</c:v>
+                  <c:v>0.10652764574884</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.102851704339032</c:v>
+                  <c:v>0.105552197299058</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.102026589839419</c:v>
+                  <c:v>0.104680229424097</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.10128916619135</c:v>
+                  <c:v>0.103900340891528</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.100629787285513</c:v>
+                  <c:v>0.103202462883249</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.100039927986691</c:v>
+                  <c:v>0.102577690206887</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.0995120433231249</c:v>
+                  <c:v>0.102018135953092</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.0990394470961825</c:v>
+                  <c:v>0.101516806058505</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.0986162069770794</c:v>
+                  <c:v>0.10106749079813</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.0982370536315273</c:v>
+                  <c:v>0.100664670704454</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.0978973018083312</c:v>
+                  <c:v>0.100303434807376</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.0975927816570149</c:v>
+                  <c:v>0.0999794094207643</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.0973197788134949</c:v>
+                  <c:v>0.0996886959786417</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.0970749820209617</c:v>
+                  <c:v>0.0994278166556479</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.0968554372432868</c:v>
+                  <c:v>0.0991936666999892</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.09665850738696</c:v>
+                  <c:v>0.0989834725690482</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.0964818368801902</c:v>
+                  <c:v>0.0987947550934689</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.0963233204688595</c:v>
+                  <c:v>0.0986252970093211</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.0961810756821891</c:v>
+                  <c:v>0.0984731142935804</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.0960534184993347</c:v>
+                  <c:v>0.0983364308186833</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.0959388418141656</c:v>
+                  <c:v>0.0982136559098817</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.0958359963512969</c:v>
+                  <c:v>0.0981033644466105</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.0957436737337276</c:v>
+                  <c:v>0.0980042791978352</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.095660791442611</c:v>
+                  <c:v>0.0979152551228005</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.095586379443905</c:v>
+                  <c:v>0.0978352654039332</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.0955195682858869</c:v>
+                  <c:v>0.0977633890088559</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.0954595784965598</c:v>
+                  <c:v>0.0976987996043527</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.0954057111314898</c:v>
+                  <c:v>0.0976407556673698</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.0953573393411466</c:v>
+                  <c:v>0.0975885916573004</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.0953139008428195</c:v>
+                  <c:v>0.0975417101303593</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.0952748911960417</c:v>
+                  <c:v>0.0974995746911939</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.0952398577924847</c:v>
+                  <c:v>0.0974617036893272</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.0952083944817524</c:v>
+                  <c:v>0.0974276645788689</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.0951801367636377</c:v>
+                  <c:v>0.0973970688693826</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.0951547574853844</c:v>
+                  <c:v>0.0973695676040637</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.0951319629894922</c:v>
+                  <c:v>0.0973448473086288</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.0951114896637405</c:v>
+                  <c:v>0.0973226263606712</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.0950931008505035</c:v>
+                  <c:v>0.0973026517348364</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.095076584077188</c:v>
+                  <c:v>0.0972846960840956</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.0950617485738187</c:v>
+                  <c:v>0.0972685551217499</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.0950484230475091</c:v>
+                  <c:v>0.0972540452726418</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.095036453686835</c:v>
+                  <c:v>0.0972410015654557</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.0950257023720388</c:v>
+                  <c:v>0.0972292757410092</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.0950160450695766</c:v>
+                  <c:v>0.0972187345541154</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.0950073703918087</c:v>
+                  <c:v>0.0972092582489774</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.0949995783046776</c:v>
+                  <c:v>0.0972007391901948</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -978,6 +982,18 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1307,304 +1323,304 @@
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0119996666666667</c:v>
+                  <c:v>0.0119666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0143858683814444</c:v>
+                  <c:v>0.0143069477777778</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0172274650510693</c:v>
+                  <c:v>0.0170861399283012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0206030210437717</c:v>
+                  <c:v>0.0203785102524293</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0246010275179598</c:v>
+                  <c:v>0.02426745586281</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0293195333216741</c:v>
+                  <c:v>0.0288451132270346</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0348648818900829</c:v>
+                  <c:v>0.0342111451932204</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0413491716354171</c:v>
+                  <c:v>0.0404703639782715</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0488859857636303</c:v>
+                  <c:v>0.0477287872355488</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.057583898700983</c:v>
+                  <c:v>0.056087692558346</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0675372989793939</c:v>
+                  <c:v>0.0656352665785961</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0788142261269239</c:v>
+                  <c:v>0.0764355837602081</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0914412651652086</c:v>
+                  <c:v>0.0885149505605168</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.105386133150505</c:v>
+                  <c:v>0.101846160504506</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.120539444539351</c:v>
+                  <c:v>0.116331939860325</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.136698184178212</c:v>
+                  <c:v>0.131789764385472</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.15355443563328</c:v>
+                  <c:v>0.147941121565474</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.170693531081693</c:v>
+                  <c:v>0.164408869274277</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.187605519996316</c:v>
+                  <c:v>0.180726192856701</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.203712275693566</c:v>
+                  <c:v>0.196359418782484</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.218409594641274</c:v>
+                  <c:v>0.21074449762178</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.231119821659249</c:v>
+                  <c:v>0.223333701185429</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.241347016634617</c:v>
+                  <c:v>0.233645908056472</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.24872488900242</c:v>
+                  <c:v>0.241311979832774</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.253048656865067</c:v>
+                  <c:v>0.246107095048682</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.254285569013606</c:v>
+                  <c:v>0.247964630565549</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.252563834416013</c:v>
+                  <c:v>0.246970391563043</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.248144336164091</c:v>
+                  <c:v>0.243340213953038</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.241382295606971</c:v>
+                  <c:v>0.237386837224267</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.232686484783408</c:v>
+                  <c:v>0.229482828431734</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.222482122570817</c:v>
+                  <c:v>0.220025437599454</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.211181204929862</c:v>
+                  <c:v>0.209407333112339</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.199161648387605</c:v>
+                  <c:v>0.197995037285949</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.186754842310712</c:v>
+                  <c:v>0.18611514387668</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.174240179321604</c:v>
+                  <c:v>0.174047292683899</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.161844760096456</c:v>
+                  <c:v>0.162022374350162</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.149746533169698</c:v>
+                  <c:v>0.15022437868476</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.13807942078182</c:v>
+                  <c:v>0.138794495852543</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.12693934322727</c:v>
+                  <c:v>0.12783638115245</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.116390395404104</c:v>
+                  <c:v>0.117421803862028</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.106470709165651</c:v>
+                  <c:v>0.107596168705287</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.0971977440057137</c:v>
+                  <c:v>0.0983836072403376</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0885728932374573</c:v>
+                  <c:v>0.0897914866420663</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.0805853860408438</c:v>
+                  <c:v>0.0818142841492325</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.0732155211016092</c:v>
+                  <c:v>0.0744368383541866</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0664372967391129</c:v>
+                  <c:v>0.0676370242806383</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.0602205145044203</c:v>
+                  <c:v>0.0613879165983053</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.0545324348061236</c:v>
+                  <c:v>0.0556595109732671</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.04933905871349</c:v>
+                  <c:v>0.0504200721457033</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.0446061026633117</c:v>
+                  <c:v>0.0456371720442725</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.0402997242184137</c:v>
+                  <c:v>0.041278474151554</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.0363870483957644</c:v>
+                  <c:v>0.0373123127033571</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.0328365360070725</c:v>
+                  <c:v>0.0337081078794776</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.0296182282263256</c:v>
+                  <c:v>0.0304366513202712</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.0267038953171669</c:v>
+                  <c:v>0.027470290259168</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.0240671121081296</c:v>
+                  <c:v>0.0247830333410611</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.0216832783266589</c:v>
+                  <c:v>0.0223505967705479</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.0195295981978404</c:v>
+                  <c:v>0.0201504057337104</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.0175850306772988</c:v>
+                  <c:v>0.018161562977494</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.0158302192191475</c:v>
+                  <c:v>0.0163647939235237</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.0142474079868269</c:v>
+                  <c:v>0.0147423756541828</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.0128203498155258</c:v>
+                  <c:v>0.0132780554615451</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.0115342099592254</c:v>
+                  <c:v>0.011956963327047</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.0103754686435474</c:v>
+                  <c:v>0.010765521643784</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.00933182464760387</c:v>
+                  <c:v>0.0096913546550239</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.00839210151257299</c:v>
+                  <c:v>0.00872319942096583</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.00754615748774994</c:v>
+                  <c:v>0.00785081960695963</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.00678479994858315</c:v>
+                  <c:v>0.0070649229823588</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.00609970473311358</c:v>
+                  <c:v>0.00635708320703637</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.00548334062502532</c:v>
+                  <c:v>0.00571966624370581</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.00492889904845835</c:v>
+                  <c:v>0.0051457615534577</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.00443022891999467</c:v>
+                  <c:v>0.00462911809714442</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.0039817765173324</c:v>
+                  <c:v>0.00416408506659919</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.00357853016454245</c:v>
+                  <c:v>0.00374555719928311</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.00321596949443922</c:v>
+                  <c:v>0.0033689244815136</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.00289001902471605</c:v>
+                  <c:v>0.00303002601391637</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.0025970057723232</c:v>
+                  <c:v>0.00272510779416951</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.00233362062713008</c:v>
+                  <c:v>0.0024507841633149</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.00209688320888542</c:v>
+                  <c:v>0.00220400266040688</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.00188410993905206</c:v>
+                  <c:v>0.00198201203409659</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.00169288506983892</c:v>
+                  <c:v>0.00178233316738692</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.00152103442559704</c:v>
+                  <c:v>0.00160273268205157</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.00136660162586062</c:v>
+                  <c:v>0.0014411990011808</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.00122782657407299</c:v>
+                  <c:v>0.00129592066129774</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.00110312601097438</c:v>
+                  <c:v>0.00116526667895679</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.000991075946401502</c:v>
+                  <c:v>0.00104776879029592</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.000890395797613579</c:v>
+                  <c:v>0.000942105395381382</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.000799934076046465</c:v>
+                  <c:v>0.000847087052150251</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.000718655477493602</c:v>
+                  <c:v>0.000761643377182432</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.00064562924305327</c:v>
+                  <c:v>0.000684811222326358</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.000580018669731194</c:v>
+                  <c:v>0.000615724007307042</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.000521071660337339</c:v>
+                  <c:v>0.00055360209883425</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.000468112212274627</c:v>
+                  <c:v>0.000497744136397198</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.000420532754007306</c:v>
+                  <c:v>0.000447519213889919</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.000377787246449164</c:v>
+                  <c:v>0.000402359834479361</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.000339384974263427</c:v>
+                  <c:v>0.000361755563734896</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.000304884959157835</c:v>
+                  <c:v>0.000325247313016729</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.000273890933732338</c:v>
+                  <c:v>0.000292422191508274</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.000246046820335913</c:v>
+                  <c:v>0.000262908871111829</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.000221032664755585</c:v>
+                  <c:v>0.000236373413746205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1644,6 +1660,18 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1976,318 +2004,318 @@
                   <c:v>0.00133333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00293328888888889</c:v>
+                  <c:v>0.00292888888888888</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00485140467308148</c:v>
+                  <c:v>0.00483648192592591</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00714840001322405</c:v>
+                  <c:v>0.00711463391636607</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.00989546948572693</c:v>
+                  <c:v>0.00983176861668997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0131756064881216</c:v>
+                  <c:v>0.013067429398398</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0170848775976781</c:v>
+                  <c:v>0.0169134444953359</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0217335285163558</c:v>
+                  <c:v>0.0214749305210986</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0272467514010781</c:v>
+                  <c:v>0.0268709790515348</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0337648828362288</c:v>
+                  <c:v>0.033234817349608</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0414427359963599</c:v>
+                  <c:v>0.0407131763573874</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0504477091936124</c:v>
+                  <c:v>0.0494645452345335</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0609562726772023</c:v>
+                  <c:v>0.0596559564025613</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0731484413658968</c:v>
+                  <c:v>0.0714579498106301</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.087199925785964</c:v>
+                  <c:v>0.0850374378778975</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.103271851724544</c:v>
+                  <c:v>0.100548363192607</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.121498276281639</c:v>
+                  <c:v>0.118120331777337</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.141972201032743</c:v>
+                  <c:v>0.137845814652733</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.164731338510302</c:v>
+                  <c:v>0.159766997222637</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.189745407843144</c:v>
+                  <c:v>0.183863822936864</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.216907044602286</c:v>
+                  <c:v>0.210045078774528</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.246028323887789</c:v>
+                  <c:v>0.238144345124099</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.276844300109022</c:v>
+                  <c:v>0.267922171948822</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.309023902326971</c:v>
+                  <c:v>0.299074959689685</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.342187220860627</c:v>
+                  <c:v>0.331249890334055</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.37592704177597</c:v>
+                  <c:v>0.364064169673879</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.409831784311117</c:v>
+                  <c:v>0.397126120415952</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.443506962233252</c:v>
+                  <c:v>0.430055505957691</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.476592873721798</c:v>
+                  <c:v>0.462500867818096</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.508777179802727</c:v>
+                  <c:v>0.494152446114665</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.539802044440515</c:v>
+                  <c:v>0.52475015657223</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.569466327449957</c:v>
+                  <c:v>0.55408688158549</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.597623821440605</c:v>
+                  <c:v>0.582007859333802</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.624178707892286</c:v>
+                  <c:v>0.608407197638595</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.649079353533714</c:v>
+                  <c:v>0.633222550155486</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.672311377443261</c:v>
+                  <c:v>0.656428855846672</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.693890678789456</c:v>
+                  <c:v>0.678031839093361</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.713856883212082</c:v>
+                  <c:v>0.698061756251328</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.732267472649658</c:v>
+                  <c:v>0.716567689031668</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.749192718413294</c:v>
+                  <c:v>0.733612539851994</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.764711437800508</c:v>
+                  <c:v>0.749268780366931</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.778907532355928</c:v>
+                  <c:v>0.763614936194303</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.79186723155669</c:v>
+                  <c:v>0.776732750493014</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.803676950655017</c:v>
+                  <c:v>0.788704948711956</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.814421668793796</c:v>
+                  <c:v>0.799613519931854</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.824183738274011</c:v>
+                  <c:v>0.809538431712412</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.833042044505893</c:v>
+                  <c:v>0.818556701616497</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.841071446439816</c:v>
+                  <c:v>0.826741757162938</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.848342437747299</c:v>
+                  <c:v>0.834163025292707</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.854920978909097</c:v>
+                  <c:v>0.840885701578801</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.860868459264206</c:v>
+                  <c:v>0.846970657851371</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.866241755826661</c:v>
+                  <c:v>0.852474454404911</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.871093362279429</c:v>
+                  <c:v>0.857449429432025</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.875471567080372</c:v>
+                  <c:v>0.861943843815956</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.879420664177216</c:v>
+                  <c:v>0.866002063991992</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.882981183552838</c:v>
+                  <c:v>0.869664769359881</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.886190131833922</c:v>
+                  <c:v>0.872969173805356</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.88908123561081</c:v>
+                  <c:v>0.875949253374762</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.891685182037189</c:v>
+                  <c:v>0.878635974139257</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.894029852794162</c:v>
+                  <c:v>0.881057515869589</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.896140548690048</c:v>
+                  <c:v>0.883239488392726</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.898040203088292</c:v>
+                  <c:v>0.88520513847995</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.899749583063695</c:v>
+                  <c:v>0.886975545874823</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.901287477724925</c:v>
+                  <c:v>0.888569807651762</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.902670873544065</c:v>
+                  <c:v>0.8900052105376</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.903915116830412</c:v>
+                  <c:v>0.89129739115827</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.905034063698755</c:v>
+                  <c:v>0.892460484414399</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.906040218030455</c:v>
+                  <c:v>0.893507260361993</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.906944858023599</c:v>
+                  <c:v>0.894449250092975</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.907758151988014</c:v>
+                  <c:v>0.895296861187246</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.908489264071351</c:v>
+                  <c:v>0.896059483353074</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.909146450611146</c:v>
+                  <c:v>0.896745584893535</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.909737147800478</c:v>
+                  <c:v>0.89736280063982</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.910268051336123</c:v>
+                  <c:v>0.897918011982034</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.910745188691395</c:v>
+                  <c:v>0.898417419608605</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.911173984623987</c:v>
+                  <c:v>0.898866609539473</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.911559320493949</c:v>
+                  <c:v>0.899270613007996</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.911905587930259</c:v>
+                  <c:v>0.899633960713885</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.912216737347209</c:v>
+                  <c:v>0.89996073193566</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.912496321775061</c:v>
+                  <c:v>0.900254598957048</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.912747536433601</c:v>
+                  <c:v>0.900518867228261</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.912973254442913</c:v>
+                  <c:v>0.900756511650579</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.913176059032992</c:v>
+                  <c:v>0.900970209341519</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.913358272583107</c:v>
+                  <c:v>0.901162369208343</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.913521982792984</c:v>
+                  <c:v>0.901335158629849</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.913669066261114</c:v>
+                  <c:v>0.901490527520377</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.913801209720634</c:v>
+                  <c:v>0.90163023002575</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.913919929160315</c:v>
+                  <c:v>0.901755844078467</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.914026587037122</c:v>
+                  <c:v>0.901868789018754</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.914122407767454</c:v>
+                  <c:v>0.901970341469045</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.914208491666528</c:v>
+                  <c:v>0.902061649632022</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.914285827489159</c:v>
+                  <c:v>0.902143746166329</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.914355303710537</c:v>
+                  <c:v>0.902217559779507</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.914417718672174</c:v>
+                  <c:v>0.90228392566436</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.914473789706041</c:v>
+                  <c:v>0.902343594892879</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.914524161338901</c:v>
+                  <c:v>0.90239724287081</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.914569412668803</c:v>
+                  <c:v>0.902445476945974</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.914610063996691</c:v>
+                  <c:v>0.902488843254376</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.914646582787855</c:v>
+                  <c:v>0.902527832879911</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.914679389030566</c:v>
+                  <c:v>0.902562887396059</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="20698467"/>
-        <c:axId val="50920419"/>
+        <c:axId val="46184266"/>
+        <c:axId val="96128160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20698467"/>
+        <c:axId val="46184266"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -2309,12 +2337,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50920419"/>
+        <c:crossAx val="96128160"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50920419"/>
+        <c:axId val="96128160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2329,7 +2357,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -2351,7 +2379,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20698467"/>
+        <c:crossAx val="46184266"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2418,9 +2446,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>634320</xdr:colOff>
+      <xdr:colOff>633960</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2429,7 +2457,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4628880" y="736200"/>
-        <a:ext cx="5758920" cy="3241800"/>
+        <a:ext cx="5758560" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2449,8 +2477,8 @@
   </sheetPr>
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2508,8 +2536,8 @@
         <v>0</v>
       </c>
       <c r="B4" s="0" t="n">
-        <f aca="false">1-0.0001</f>
-        <v>0.9999</v>
+        <f aca="false">1-0.01</f>
+        <v>0.99</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>0.01</v>
@@ -2519,7 +2547,7 @@
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">B4+C4+D4</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,11 +2556,11 @@
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">B4-H$1*B4*C4</f>
-        <v>0.996567</v>
+        <v>0.9867</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">C4+H$1*B4*C4-F$1*C4</f>
-        <v>0.0119996666666667</v>
+        <v>0.0119666666666667</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">D4+F$1*C4</f>
@@ -2540,7 +2568,7 @@
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">B5+C5+D5</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2549,19 +2577,19 @@
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">B5-H$1*B5*C5</f>
-        <v>0.992580842729667</v>
+        <v>0.982764163333333</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">C5+H$1*B5*C5-F$1*C5</f>
-        <v>0.0143858683814444</v>
+        <v>0.0143069477777778</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">D5+F$1*C5</f>
-        <v>0.00293328888888889</v>
+        <v>0.00292888888888888</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">B6+C6+D6</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2570,19 +2598,19 @@
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B6-H$1*B6*C6</f>
-        <v>0.987821130275849</v>
+        <v>0.978077378145773</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">C6+H$1*B6*C6-F$1*C6</f>
-        <v>0.0172274650510693</v>
+        <v>0.0170861399283012</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">D6+F$1*C6</f>
-        <v>0.00485140467308148</v>
+        <v>0.00483648192592591</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">B7+C7+D7</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2591,19 +2619,19 @@
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B7-H$1*B7*C7</f>
-        <v>0.982148578943004</v>
+        <v>0.972506855831205</v>
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">C7+H$1*B7*C7-F$1*C7</f>
-        <v>0.0206030210437717</v>
+        <v>0.0203785102524293</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">D7+F$1*C7</f>
-        <v>0.00714840001322405</v>
+        <v>0.00711463391636607</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">B8+C8+D8</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2612,19 +2640,19 @@
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B8-H$1*B8*C8</f>
-        <v>0.975403502996313</v>
+        <v>0.9659007755205</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">C8+H$1*B8*C8-F$1*C8</f>
-        <v>0.0246010275179598</v>
+        <v>0.02426745586281</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">D8+F$1*C8</f>
-        <v>0.00989546948572693</v>
+        <v>0.00983176861668997</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">B9+C9+D9</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2633,19 +2661,19 @@
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B9-H$1*B9*C9</f>
-        <v>0.967404860190204</v>
+        <v>0.958087457374567</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">C9+H$1*B9*C9-F$1*C9</f>
-        <v>0.0293195333216741</v>
+        <v>0.0288451132270346</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">D9+F$1*C9</f>
-        <v>0.0131756064881216</v>
+        <v>0.013067429398398</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">B10+C10+D10</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2654,19 +2682,19 @@
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10-H$1*B10*C10</f>
-        <v>0.957950240512239</v>
+        <v>0.948875410311444</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">C10+H$1*B10*C10-F$1*C10</f>
-        <v>0.0348648818900829</v>
+        <v>0.0342111451932204</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">D10+F$1*C10</f>
-        <v>0.0170848775976781</v>
+        <v>0.0169134444953359</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">B11+C11+D11</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2675,19 +2703,19 @@
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">B11-H$1*B11*C11</f>
-        <v>0.946817299848227</v>
+        <v>0.93805470550063</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">C11+H$1*B11*C11-F$1*C11</f>
-        <v>0.0413491716354171</v>
+        <v>0.0404703639782715</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">D11+F$1*C11</f>
-        <v>0.0217335285163558</v>
+        <v>0.0214749305210986</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">B12+C12+D12</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,19 +2724,19 @@
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">B12-H$1*B12*C12</f>
-        <v>0.933767262835291</v>
+        <v>0.925400233712916</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">C12+H$1*B12*C12-F$1*C12</f>
-        <v>0.0488859857636303</v>
+        <v>0.0477287872355488</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">D12+F$1*C12</f>
-        <v>0.0272467514010781</v>
+        <v>0.0268709790515348</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">B13+C13+D13</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,19 +2745,19 @@
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">B13-H$1*B13*C13</f>
-        <v>0.918551218462788</v>
+        <v>0.910677490092046</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">C13+H$1*B13*C13-F$1*C13</f>
-        <v>0.057583898700983</v>
+        <v>0.056087692558346</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">D13+F$1*C13</f>
-        <v>0.0337648828362288</v>
+        <v>0.033234817349608</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">B14+C14+D14</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2738,19 +2766,19 @@
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">B14-H$1*B14*C14</f>
-        <v>0.900919965024246</v>
+        <v>0.893651557064016</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">C14+H$1*B14*C14-F$1*C14</f>
-        <v>0.0675372989793939</v>
+        <v>0.0656352665785961</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">D14+F$1*C14</f>
-        <v>0.0414427359963599</v>
+        <v>0.0407131763573874</v>
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">B15+C15+D15</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2759,19 +2787,19 @@
       </c>
       <c r="B16" s="0" t="n">
         <f aca="false">B15-H$1*B15*C15</f>
-        <v>0.880638064679464</v>
+        <v>0.874099871005258</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">C15+H$1*B15*C15-F$1*C15</f>
-        <v>0.0788142261269239</v>
+        <v>0.0764355837602081</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">D15+F$1*C15</f>
-        <v>0.0504477091936124</v>
+        <v>0.0494645452345335</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">B16+C16+D16</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2780,19 +2808,19 @@
       </c>
       <c r="B17" s="0" t="n">
         <f aca="false">B16-H$1*B16*C16</f>
-        <v>0.857502462157589</v>
+        <v>0.851829093036922</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">C16+H$1*B16*C16-F$1*C16</f>
-        <v>0.0914412651652086</v>
+        <v>0.0885149505605168</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">D16+F$1*C16</f>
-        <v>0.0609562726772023</v>
+        <v>0.0596559564025613</v>
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">B17+C17+D17</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2801,19 +2829,19 @@
       </c>
       <c r="B18" s="0" t="n">
         <f aca="false">B17-H$1*B17*C17</f>
-        <v>0.831365425483599</v>
+        <v>0.826695889684864</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">C17+H$1*B17*C17-F$1*C17</f>
-        <v>0.105386133150505</v>
+        <v>0.101846160504506</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">D17+F$1*C17</f>
-        <v>0.0731484413658968</v>
+        <v>0.0714579498106301</v>
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">B18+C18+D18</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2822,19 +2850,19 @@
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">B18-H$1*B18*C18</f>
-        <v>0.802160629674685</v>
+        <v>0.798630622261778</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">C18+H$1*B18*C18-F$1*C18</f>
-        <v>0.120539444539351</v>
+        <v>0.116331939860325</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">D18+F$1*C18</f>
-        <v>0.087199925785964</v>
+        <v>0.0850374378778975</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">B19+C19+D19</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2843,19 +2871,19 @@
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">B19-H$1*B19*C19</f>
-        <v>0.769929964097244</v>
+        <v>0.767661872421921</v>
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">C19+H$1*B19*C19-F$1*C19</f>
-        <v>0.136698184178212</v>
+        <v>0.131789764385472</v>
       </c>
       <c r="D20" s="0" t="n">
         <f aca="false">D19+F$1*C19</f>
-        <v>0.103271851724544</v>
+        <v>0.100548363192607</v>
       </c>
       <c r="E20" s="0" t="n">
         <f aca="false">B20+C20+D20</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2864,19 +2892,19 @@
       </c>
       <c r="B21" s="0" t="n">
         <f aca="false">B20-H$1*B20*C20</f>
-        <v>0.734847288085081</v>
+        <v>0.733938546657189</v>
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">C20+H$1*B20*C20-F$1*C20</f>
-        <v>0.15355443563328</v>
+        <v>0.147941121565474</v>
       </c>
       <c r="D21" s="0" t="n">
         <f aca="false">D20+F$1*C20</f>
-        <v>0.121498276281639</v>
+        <v>0.118120331777337</v>
       </c>
       <c r="E21" s="0" t="n">
         <f aca="false">B21+C21+D21</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2885,19 +2913,19 @@
       </c>
       <c r="B22" s="0" t="n">
         <f aca="false">B21-H$1*B21*C21</f>
-        <v>0.697234267885565</v>
+        <v>0.69774531607299</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">C21+H$1*B21*C21-F$1*C21</f>
-        <v>0.170693531081693</v>
+        <v>0.164408869274277</v>
       </c>
       <c r="D22" s="0" t="n">
         <f aca="false">D21+F$1*C21</f>
-        <v>0.141972201032743</v>
+        <v>0.137845814652733</v>
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">B22+C22+D22</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2906,19 +2934,19 @@
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B22-H$1*B22*C22</f>
-        <v>0.657563141493383</v>
+        <v>0.659506809920662</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">C22+H$1*B22*C22-F$1*C22</f>
-        <v>0.187605519996316</v>
+        <v>0.180726192856701</v>
       </c>
       <c r="D23" s="0" t="n">
         <f aca="false">D22+F$1*C22</f>
-        <v>0.164731338510302</v>
+        <v>0.159766997222637</v>
       </c>
       <c r="E23" s="0" t="n">
         <f aca="false">B23+C23+D23</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2927,19 +2955,19 @@
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">B23-H$1*B23*C23</f>
-        <v>0.61644231646329</v>
+        <v>0.619776758280652</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">C23+H$1*B23*C23-F$1*C23</f>
-        <v>0.203712275693566</v>
+        <v>0.196359418782484</v>
       </c>
       <c r="D24" s="0" t="n">
         <f aca="false">D23+F$1*C23</f>
-        <v>0.189745407843144</v>
+        <v>0.183863822936864</v>
       </c>
       <c r="E24" s="0" t="n">
         <f aca="false">B24+C24+D24</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2948,19 +2976,19 @@
       </c>
       <c r="B25" s="0" t="n">
         <f aca="false">B24-H$1*B24*C24</f>
-        <v>0.57458336075644</v>
+        <v>0.579210423603692</v>
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">C24+H$1*B24*C24-F$1*C24</f>
-        <v>0.218409594641274</v>
+        <v>0.21074449762178</v>
       </c>
       <c r="D25" s="0" t="n">
         <f aca="false">D24+F$1*C24</f>
-        <v>0.216907044602286</v>
+        <v>0.210045078774528</v>
       </c>
       <c r="E25" s="0" t="n">
         <f aca="false">B25+C25+D25</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2969,19 +2997,19 @@
       </c>
       <c r="B26" s="0" t="n">
         <f aca="false">B25-H$1*B25*C25</f>
-        <v>0.532751854452962</v>
+        <v>0.538521953690473</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">C25+H$1*B25*C25-F$1*C25</f>
-        <v>0.231119821659249</v>
+        <v>0.223333701185429</v>
       </c>
       <c r="D26" s="0" t="n">
         <f aca="false">D25+F$1*C25</f>
-        <v>0.246028323887789</v>
+        <v>0.238144345124099</v>
       </c>
       <c r="E26" s="0" t="n">
         <f aca="false">B26+C26+D26</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2990,19 +3018,19 @@
       </c>
       <c r="B27" s="0" t="n">
         <f aca="false">B26-H$1*B26*C26</f>
-        <v>0.491708683256361</v>
+        <v>0.498431919994706</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">C26+H$1*B26*C26-F$1*C26</f>
-        <v>0.241347016634617</v>
+        <v>0.233645908056472</v>
       </c>
       <c r="D27" s="0" t="n">
         <f aca="false">D26+F$1*C26</f>
-        <v>0.276844300109022</v>
+        <v>0.267922171948822</v>
       </c>
       <c r="E27" s="0" t="n">
         <f aca="false">B27+C27+D27</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3011,19 +3039,19 @@
       </c>
       <c r="B28" s="0" t="n">
         <f aca="false">B27-H$1*B27*C27</f>
-        <v>0.452151208670608</v>
+        <v>0.459613060477541</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">C27+H$1*B27*C27-F$1*C27</f>
-        <v>0.24872488900242</v>
+        <v>0.241311979832774</v>
       </c>
       <c r="D28" s="0" t="n">
         <f aca="false">D27+F$1*C27</f>
-        <v>0.309023902326971</v>
+        <v>0.299074959689685</v>
       </c>
       <c r="E28" s="0" t="n">
         <f aca="false">B28+C28+D28</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3032,19 +3060,19 @@
       </c>
       <c r="B29" s="0" t="n">
         <f aca="false">B28-H$1*B28*C28</f>
-        <v>0.414664122274306</v>
+        <v>0.422643014617262</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">C28+H$1*B28*C28-F$1*C28</f>
-        <v>0.253048656865067</v>
+        <v>0.246107095048682</v>
       </c>
       <c r="D29" s="0" t="n">
         <f aca="false">D28+F$1*C28</f>
-        <v>0.342187220860627</v>
+        <v>0.331249890334055</v>
       </c>
       <c r="E29" s="0" t="n">
         <f aca="false">B29+C29+D29</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,19 +3081,19 @@
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">B29-H$1*B29*C29</f>
-        <v>0.379687389210424</v>
+        <v>0.387971199760572</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C29+H$1*B29*C29-F$1*C29</f>
-        <v>0.254285569013606</v>
+        <v>0.247964630565549</v>
       </c>
       <c r="D30" s="0" t="n">
         <f aca="false">D29+F$1*C29</f>
-        <v>0.37592704177597</v>
+        <v>0.364064169673879</v>
       </c>
       <c r="E30" s="0" t="n">
         <f aca="false">B30+C30+D30</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3074,19 +3102,19 @@
       </c>
       <c r="B31" s="0" t="n">
         <f aca="false">B30-H$1*B30*C30</f>
-        <v>0.34750438127287</v>
+        <v>0.355903488021004</v>
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">C30+H$1*B30*C30-F$1*C30</f>
-        <v>0.252563834416013</v>
+        <v>0.246970391563043</v>
       </c>
       <c r="D31" s="0" t="n">
         <f aca="false">D30+F$1*C30</f>
-        <v>0.409831784311117</v>
+        <v>0.397126120415952</v>
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">B31+C31+D31</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3095,19 +3123,19 @@
       </c>
       <c r="B32" s="0" t="n">
         <f aca="false">B31-H$1*B31*C31</f>
-        <v>0.318248701602656</v>
+        <v>0.326604280089271</v>
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">C31+H$1*B31*C31-F$1*C31</f>
-        <v>0.248144336164091</v>
+        <v>0.243340213953038</v>
       </c>
       <c r="D32" s="0" t="n">
         <f aca="false">D31+F$1*C31</f>
-        <v>0.443506962233252</v>
+        <v>0.430055505957691</v>
       </c>
       <c r="E32" s="0" t="n">
         <f aca="false">B32+C32+D32</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3116,19 +3144,19 @@
       </c>
       <c r="B33" s="0" t="n">
         <f aca="false">B32-H$1*B32*C32</f>
-        <v>0.291924830671231</v>
+        <v>0.300112294957637</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C32+H$1*B32*C32-F$1*C32</f>
-        <v>0.241382295606971</v>
+        <v>0.237386837224267</v>
       </c>
       <c r="D33" s="0" t="n">
         <f aca="false">D32+F$1*C32</f>
-        <v>0.476592873721798</v>
+        <v>0.462500867818096</v>
       </c>
       <c r="E33" s="0" t="n">
         <f aca="false">B33+C33+D33</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3137,19 +3165,19 @@
       </c>
       <c r="B34" s="0" t="n">
         <f aca="false">B33-H$1*B33*C33</f>
-        <v>0.268436335413865</v>
+        <v>0.2763647254536</v>
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">C33+H$1*B33*C33-F$1*C33</f>
-        <v>0.232686484783408</v>
+        <v>0.229482828431734</v>
       </c>
       <c r="D34" s="0" t="n">
         <f aca="false">D33+F$1*C33</f>
-        <v>0.508777179802727</v>
+        <v>0.494152446114665</v>
       </c>
       <c r="E34" s="0" t="n">
         <f aca="false">B34+C34+D34</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3158,19 +3186,19 @@
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B34-H$1*B34*C34</f>
-        <v>0.247615832988668</v>
+        <v>0.255224405828316</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C34+H$1*B34*C34-F$1*C34</f>
-        <v>0.222482122570817</v>
+        <v>0.220025437599454</v>
       </c>
       <c r="D35" s="0" t="n">
         <f aca="false">D34+F$1*C34</f>
-        <v>0.539802044440515</v>
+        <v>0.52475015657223</v>
       </c>
       <c r="E35" s="0" t="n">
         <f aca="false">B35+C35+D35</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3179,19 +3207,19 @@
       </c>
       <c r="B36" s="0" t="n">
         <f aca="false">B35-H$1*B35*C35</f>
-        <v>0.229252467620181</v>
+        <v>0.236505785302171</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C35+H$1*B35*C35-F$1*C35</f>
-        <v>0.211181204929862</v>
+        <v>0.209407333112339</v>
       </c>
       <c r="D36" s="0" t="n">
         <f aca="false">D35+F$1*C35</f>
-        <v>0.569466327449957</v>
+        <v>0.55408688158549</v>
       </c>
       <c r="E36" s="0" t="n">
         <f aca="false">B36+C36+D36</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3200,19 +3228,19 @@
       </c>
       <c r="B37" s="0" t="n">
         <f aca="false">B36-H$1*B36*C36</f>
-        <v>0.21311453017179</v>
+        <v>0.219997103380249</v>
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">C36+H$1*B36*C36-F$1*C36</f>
-        <v>0.199161648387605</v>
+        <v>0.197995037285949</v>
       </c>
       <c r="D37" s="0" t="n">
         <f aca="false">D36+F$1*C36</f>
-        <v>0.597623821440605</v>
+        <v>0.582007859333802</v>
       </c>
       <c r="E37" s="0" t="n">
         <f aca="false">B37+C37+D37</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3221,19 +3249,19 @@
       </c>
       <c r="B38" s="0" t="n">
         <f aca="false">B37-H$1*B37*C37</f>
-        <v>0.198966449797002</v>
+        <v>0.205477658484725</v>
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">C37+H$1*B37*C37-F$1*C37</f>
-        <v>0.186754842310712</v>
+        <v>0.18611514387668</v>
       </c>
       <c r="D38" s="0" t="n">
         <f aca="false">D37+F$1*C37</f>
-        <v>0.624178707892286</v>
+        <v>0.608407197638595</v>
       </c>
       <c r="E38" s="0" t="n">
         <f aca="false">B38+C38+D38</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3242,19 +3270,19 @@
       </c>
       <c r="B39" s="0" t="n">
         <f aca="false">B38-H$1*B38*C38</f>
-        <v>0.186580467144682</v>
+        <v>0.192730157160615</v>
       </c>
       <c r="C39" s="0" t="n">
         <f aca="false">C38+H$1*B38*C38-F$1*C38</f>
-        <v>0.174240179321604</v>
+        <v>0.174047292683899</v>
       </c>
       <c r="D39" s="0" t="n">
         <f aca="false">D38+F$1*C38</f>
-        <v>0.649079353533714</v>
+        <v>0.633222550155486</v>
       </c>
       <c r="E39" s="0" t="n">
         <f aca="false">B39+C39+D39</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,19 +3291,19 @@
       </c>
       <c r="B40" s="0" t="n">
         <f aca="false">B39-H$1*B39*C39</f>
-        <v>0.175743862460282</v>
+        <v>0.181548769803166</v>
       </c>
       <c r="C40" s="0" t="n">
         <f aca="false">C39+H$1*B39*C39-F$1*C39</f>
-        <v>0.161844760096456</v>
+        <v>0.162022374350162</v>
       </c>
       <c r="D40" s="0" t="n">
         <f aca="false">D39+F$1*C39</f>
-        <v>0.672311377443261</v>
+        <v>0.656428855846672</v>
       </c>
       <c r="E40" s="0" t="n">
         <f aca="false">B40+C40+D40</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3284,19 +3312,19 @@
       </c>
       <c r="B41" s="0" t="n">
         <f aca="false">B40-H$1*B40*C40</f>
-        <v>0.166262788040846</v>
+        <v>0.171743782221879</v>
       </c>
       <c r="C41" s="0" t="n">
         <f aca="false">C40+H$1*B40*C40-F$1*C40</f>
-        <v>0.149746533169698</v>
+        <v>0.15022437868476</v>
       </c>
       <c r="D41" s="0" t="n">
         <f aca="false">D40+F$1*C40</f>
-        <v>0.693890678789456</v>
+        <v>0.678031839093361</v>
       </c>
       <c r="E41" s="0" t="n">
         <f aca="false">B41+C41+D41</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3305,19 +3333,19 @@
       </c>
       <c r="B42" s="0" t="n">
         <f aca="false">B41-H$1*B41*C41</f>
-        <v>0.157963696006098</v>
+        <v>0.163143747896129</v>
       </c>
       <c r="C42" s="0" t="n">
         <f aca="false">C41+H$1*B41*C41-F$1*C41</f>
-        <v>0.13807942078182</v>
+        <v>0.138794495852543</v>
       </c>
       <c r="D42" s="0" t="n">
         <f aca="false">D41+F$1*C41</f>
-        <v>0.713856883212082</v>
+        <v>0.698061756251328</v>
       </c>
       <c r="E42" s="0" t="n">
         <f aca="false">B42+C42+D42</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3326,19 +3354,19 @@
       </c>
       <c r="B43" s="0" t="n">
         <f aca="false">B42-H$1*B42*C42</f>
-        <v>0.150693184123072</v>
+        <v>0.155595929815883</v>
       </c>
       <c r="C43" s="0" t="n">
         <f aca="false">C42+H$1*B42*C42-F$1*C42</f>
-        <v>0.12693934322727</v>
+        <v>0.12783638115245</v>
       </c>
       <c r="D43" s="0" t="n">
         <f aca="false">D42+F$1*C42</f>
-        <v>0.732267472649658</v>
+        <v>0.716567689031668</v>
       </c>
       <c r="E43" s="0" t="n">
         <f aca="false">B43+C43+D43</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3347,19 +3375,19 @@
       </c>
       <c r="B44" s="0" t="n">
         <f aca="false">B43-H$1*B43*C43</f>
-        <v>0.144316886182602</v>
+        <v>0.148965656285978</v>
       </c>
       <c r="C44" s="0" t="n">
         <f aca="false">C43+H$1*B43*C43-F$1*C43</f>
-        <v>0.116390395404104</v>
+        <v>0.117421803862028</v>
       </c>
       <c r="D44" s="0" t="n">
         <f aca="false">D43+F$1*C43</f>
-        <v>0.749192718413294</v>
+        <v>0.733612539851994</v>
       </c>
       <c r="E44" s="0" t="n">
         <f aca="false">B44+C44+D44</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3368,19 +3396,19 @@
       </c>
       <c r="B45" s="0" t="n">
         <f aca="false">B44-H$1*B44*C44</f>
-        <v>0.138717853033841</v>
+        <v>0.143135050927782</v>
       </c>
       <c r="C45" s="0" t="n">
         <f aca="false">C44+H$1*B44*C44-F$1*C44</f>
-        <v>0.106470709165651</v>
+        <v>0.107596168705287</v>
       </c>
       <c r="D45" s="0" t="n">
         <f aca="false">D44+F$1*C44</f>
-        <v>0.764711437800508</v>
+        <v>0.749268780366931</v>
       </c>
       <c r="E45" s="0" t="n">
         <f aca="false">B45+C45+D45</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3389,19 +3417,19 @@
       </c>
       <c r="B46" s="0" t="n">
         <f aca="false">B45-H$1*B45*C45</f>
-        <v>0.133794723638358</v>
+        <v>0.13800145656536</v>
       </c>
       <c r="C46" s="0" t="n">
         <f aca="false">C45+H$1*B45*C45-F$1*C45</f>
-        <v>0.0971977440057137</v>
+        <v>0.0983836072403376</v>
       </c>
       <c r="D46" s="0" t="n">
         <f aca="false">D45+F$1*C45</f>
-        <v>0.778907532355928</v>
+        <v>0.763614936194303</v>
       </c>
       <c r="E46" s="0" t="n">
         <f aca="false">B46+C46+D46</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3410,19 +3438,19 @@
       </c>
       <c r="B47" s="0" t="n">
         <f aca="false">B46-H$1*B46*C46</f>
-        <v>0.129459875205853</v>
+        <v>0.13347576286492</v>
       </c>
       <c r="C47" s="0" t="n">
         <f aca="false">C46+H$1*B46*C46-F$1*C46</f>
-        <v>0.0885728932374573</v>
+        <v>0.0897914866420663</v>
       </c>
       <c r="D47" s="0" t="n">
         <f aca="false">D46+F$1*C46</f>
-        <v>0.79186723155669</v>
+        <v>0.776732750493014</v>
       </c>
       <c r="E47" s="0" t="n">
         <f aca="false">B47+C47+D47</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3431,19 +3459,19 @@
       </c>
       <c r="B48" s="0" t="n">
         <f aca="false">B47-H$1*B47*C47</f>
-        <v>0.125637663304139</v>
+        <v>0.129480767138811</v>
       </c>
       <c r="C48" s="0" t="n">
         <f aca="false">C47+H$1*B47*C47-F$1*C47</f>
-        <v>0.0805853860408438</v>
+        <v>0.0818142841492325</v>
       </c>
       <c r="D48" s="0" t="n">
         <f aca="false">D47+F$1*C47</f>
-        <v>0.803676950655017</v>
+        <v>0.788704948711956</v>
       </c>
       <c r="E48" s="0" t="n">
         <f aca="false">B48+C48+D48</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3452,19 +3480,19 @@
       </c>
       <c r="B49" s="0" t="n">
         <f aca="false">B48-H$1*B48*C48</f>
-        <v>0.122262810104594</v>
+        <v>0.125949641713959</v>
       </c>
       <c r="C49" s="0" t="n">
         <f aca="false">C48+H$1*B48*C48-F$1*C48</f>
-        <v>0.0732155211016092</v>
+        <v>0.0744368383541866</v>
       </c>
       <c r="D49" s="0" t="n">
         <f aca="false">D48+F$1*C48</f>
-        <v>0.814421668793796</v>
+        <v>0.799613519931854</v>
       </c>
       <c r="E49" s="0" t="n">
         <f aca="false">B49+C49+D49</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3473,19 +3501,19 @@
       </c>
       <c r="B50" s="0" t="n">
         <f aca="false">B49-H$1*B49*C49</f>
-        <v>0.119278964986876</v>
+        <v>0.12282454400695</v>
       </c>
       <c r="C50" s="0" t="n">
         <f aca="false">C49+H$1*B49*C49-F$1*C49</f>
-        <v>0.0664372967391129</v>
+        <v>0.0676370242806383</v>
       </c>
       <c r="D50" s="0" t="n">
         <f aca="false">D49+F$1*C49</f>
-        <v>0.824183738274011</v>
+        <v>0.809538431712412</v>
       </c>
       <c r="E50" s="0" t="n">
         <f aca="false">B50+C50+D50</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3494,19 +3522,19 @@
       </c>
       <c r="B51" s="0" t="n">
         <f aca="false">B50-H$1*B50*C50</f>
-        <v>0.116637440989687</v>
+        <v>0.120055381785197</v>
       </c>
       <c r="C51" s="0" t="n">
         <f aca="false">C50+H$1*B50*C50-F$1*C50</f>
-        <v>0.0602205145044203</v>
+        <v>0.0613879165983053</v>
       </c>
       <c r="D51" s="0" t="n">
         <f aca="false">D50+F$1*C50</f>
-        <v>0.833042044505893</v>
+        <v>0.818556701616497</v>
       </c>
       <c r="E51" s="0" t="n">
         <f aca="false">B51+C51+D51</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3515,19 +3543,19 @@
       </c>
       <c r="B52" s="0" t="n">
         <f aca="false">B51-H$1*B51*C51</f>
-        <v>0.114296118754061</v>
+        <v>0.117598731863795</v>
       </c>
       <c r="C52" s="0" t="n">
         <f aca="false">C51+H$1*B51*C51-F$1*C51</f>
-        <v>0.0545324348061236</v>
+        <v>0.0556595109732671</v>
       </c>
       <c r="D52" s="0" t="n">
         <f aca="false">D51+F$1*C51</f>
-        <v>0.841071446439816</v>
+        <v>0.826741757162938</v>
       </c>
       <c r="E52" s="0" t="n">
         <f aca="false">B52+C52+D52</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3536,19 +3564,19 @@
       </c>
       <c r="B53" s="0" t="n">
         <f aca="false">B52-H$1*B52*C52</f>
-        <v>0.112218503539211</v>
+        <v>0.11541690256159</v>
       </c>
       <c r="C53" s="0" t="n">
         <f aca="false">C52+H$1*B52*C52-F$1*C52</f>
-        <v>0.04933905871349</v>
+        <v>0.0504200721457033</v>
       </c>
       <c r="D53" s="0" t="n">
         <f aca="false">D52+F$1*C52</f>
-        <v>0.848342437747299</v>
+        <v>0.834163025292707</v>
       </c>
       <c r="E53" s="0" t="n">
         <f aca="false">B53+C53+D53</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3557,19 +3585,19 @@
       </c>
       <c r="B54" s="0" t="n">
         <f aca="false">B53-H$1*B53*C53</f>
-        <v>0.110372918427591</v>
+        <v>0.113477126376927</v>
       </c>
       <c r="C54" s="0" t="n">
         <f aca="false">C53+H$1*B53*C53-F$1*C53</f>
-        <v>0.0446061026633117</v>
+        <v>0.0456371720442725</v>
       </c>
       <c r="D54" s="0" t="n">
         <f aca="false">D53+F$1*C53</f>
-        <v>0.854920978909097</v>
+        <v>0.840885701578801</v>
       </c>
       <c r="E54" s="0" t="n">
         <f aca="false">B54+C54+D54</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3578,19 +3606,19 @@
       </c>
       <c r="B55" s="0" t="n">
         <f aca="false">B54-H$1*B54*C54</f>
-        <v>0.108731816517381</v>
+        <v>0.111750867997076</v>
       </c>
       <c r="C55" s="0" t="n">
         <f aca="false">C54+H$1*B54*C54-F$1*C54</f>
-        <v>0.0402997242184137</v>
+        <v>0.041278474151554</v>
       </c>
       <c r="D55" s="0" t="n">
         <f aca="false">D54+F$1*C54</f>
-        <v>0.860868459264206</v>
+        <v>0.846970657851371</v>
       </c>
       <c r="E55" s="0" t="n">
         <f aca="false">B55+C55+D55</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3599,19 +3627,19 @@
       </c>
       <c r="B56" s="0" t="n">
         <f aca="false">B55-H$1*B55*C55</f>
-        <v>0.107271195777575</v>
+        <v>0.110213232891732</v>
       </c>
       <c r="C56" s="0" t="n">
         <f aca="false">C55+H$1*B55*C55-F$1*C55</f>
-        <v>0.0363870483957644</v>
+        <v>0.0373123127033571</v>
       </c>
       <c r="D56" s="0" t="n">
         <f aca="false">D55+F$1*C55</f>
-        <v>0.866241755826661</v>
+        <v>0.852474454404911</v>
       </c>
       <c r="E56" s="0" t="n">
         <f aca="false">B56+C56+D56</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3620,19 +3648,19 @@
       </c>
       <c r="B57" s="0" t="n">
         <f aca="false">B56-H$1*B56*C56</f>
-        <v>0.105970101713498</v>
+        <v>0.108842462688497</v>
       </c>
       <c r="C57" s="0" t="n">
         <f aca="false">C56+H$1*B56*C56-F$1*C56</f>
-        <v>0.0328365360070725</v>
+        <v>0.0337081078794776</v>
       </c>
       <c r="D57" s="0" t="n">
         <f aca="false">D56+F$1*C56</f>
-        <v>0.871093362279429</v>
+        <v>0.857449429432025</v>
       </c>
       <c r="E57" s="0" t="n">
         <f aca="false">B57+C57+D57</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3641,19 +3669,19 @@
       </c>
       <c r="B58" s="0" t="n">
         <f aca="false">B57-H$1*B57*C57</f>
-        <v>0.104810204693302</v>
+        <v>0.107619504863773</v>
       </c>
       <c r="C58" s="0" t="n">
         <f aca="false">C57+H$1*B57*C57-F$1*C57</f>
-        <v>0.0296182282263256</v>
+        <v>0.0304366513202712</v>
       </c>
       <c r="D58" s="0" t="n">
         <f aca="false">D57+F$1*C57</f>
-        <v>0.875471567080372</v>
+        <v>0.861943843815956</v>
       </c>
       <c r="E58" s="0" t="n">
         <f aca="false">B58+C58+D58</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3662,19 +3690,19 @@
       </c>
       <c r="B59" s="0" t="n">
         <f aca="false">B58-H$1*B58*C58</f>
-        <v>0.103775440505617</v>
+        <v>0.10652764574884</v>
       </c>
       <c r="C59" s="0" t="n">
         <f aca="false">C58+H$1*B58*C58-F$1*C58</f>
-        <v>0.0267038953171669</v>
+        <v>0.027470290259168</v>
       </c>
       <c r="D59" s="0" t="n">
         <f aca="false">D58+F$1*C58</f>
-        <v>0.879420664177216</v>
+        <v>0.866002063991992</v>
       </c>
       <c r="E59" s="0" t="n">
         <f aca="false">B59+C59+D59</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3683,19 +3711,19 @@
       </c>
       <c r="B60" s="0" t="n">
         <f aca="false">B59-H$1*B59*C59</f>
-        <v>0.102851704339032</v>
+        <v>0.105552197299058</v>
       </c>
       <c r="C60" s="0" t="n">
         <f aca="false">C59+H$1*B59*C59-F$1*C59</f>
-        <v>0.0240671121081296</v>
+        <v>0.0247830333410611</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">D59+F$1*C59</f>
-        <v>0.882981183552838</v>
+        <v>0.869664769359881</v>
       </c>
       <c r="E60" s="0" t="n">
         <f aca="false">B60+C60+D60</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3704,19 +3732,19 @@
       </c>
       <c r="B61" s="0" t="n">
         <f aca="false">B60-H$1*B60*C60</f>
-        <v>0.102026589839419</v>
+        <v>0.104680229424097</v>
       </c>
       <c r="C61" s="0" t="n">
         <f aca="false">C60+H$1*B60*C60-F$1*C60</f>
-        <v>0.0216832783266589</v>
+        <v>0.0223505967705479</v>
       </c>
       <c r="D61" s="0" t="n">
         <f aca="false">D60+F$1*C60</f>
-        <v>0.886190131833922</v>
+        <v>0.872969173805356</v>
       </c>
       <c r="E61" s="0" t="n">
         <f aca="false">B61+C61+D61</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3725,19 +3753,19 @@
       </c>
       <c r="B62" s="0" t="n">
         <f aca="false">B61-H$1*B61*C61</f>
-        <v>0.10128916619135</v>
+        <v>0.103900340891528</v>
       </c>
       <c r="C62" s="0" t="n">
         <f aca="false">C61+H$1*B61*C61-F$1*C61</f>
-        <v>0.0195295981978404</v>
+        <v>0.0201504057337104</v>
       </c>
       <c r="D62" s="0" t="n">
         <f aca="false">D61+F$1*C61</f>
-        <v>0.88908123561081</v>
+        <v>0.875949253374762</v>
       </c>
       <c r="E62" s="0" t="n">
         <f aca="false">B62+C62+D62</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3746,19 +3774,19 @@
       </c>
       <c r="B63" s="0" t="n">
         <f aca="false">B62-H$1*B62*C62</f>
-        <v>0.100629787285513</v>
+        <v>0.103202462883249</v>
       </c>
       <c r="C63" s="0" t="n">
         <f aca="false">C62+H$1*B62*C62-F$1*C62</f>
-        <v>0.0175850306772988</v>
+        <v>0.018161562977494</v>
       </c>
       <c r="D63" s="0" t="n">
         <f aca="false">D62+F$1*C62</f>
-        <v>0.891685182037189</v>
+        <v>0.878635974139257</v>
       </c>
       <c r="E63" s="0" t="n">
         <f aca="false">B63+C63+D63</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3767,19 +3795,19 @@
       </c>
       <c r="B64" s="0" t="n">
         <f aca="false">B63-H$1*B63*C63</f>
-        <v>0.100039927986691</v>
+        <v>0.102577690206887</v>
       </c>
       <c r="C64" s="0" t="n">
         <f aca="false">C63+H$1*B63*C63-F$1*C63</f>
-        <v>0.0158302192191475</v>
+        <v>0.0163647939235237</v>
       </c>
       <c r="D64" s="0" t="n">
         <f aca="false">D63+F$1*C63</f>
-        <v>0.894029852794162</v>
+        <v>0.881057515869589</v>
       </c>
       <c r="E64" s="0" t="n">
         <f aca="false">B64+C64+D64</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3788,19 +3816,19 @@
       </c>
       <c r="B65" s="0" t="n">
         <f aca="false">B64-H$1*B64*C64</f>
-        <v>0.0995120433231249</v>
+        <v>0.102018135953092</v>
       </c>
       <c r="C65" s="0" t="n">
         <f aca="false">C64+H$1*B64*C64-F$1*C64</f>
-        <v>0.0142474079868269</v>
+        <v>0.0147423756541828</v>
       </c>
       <c r="D65" s="0" t="n">
         <f aca="false">D64+F$1*C64</f>
-        <v>0.896140548690048</v>
+        <v>0.883239488392726</v>
       </c>
       <c r="E65" s="0" t="n">
         <f aca="false">B65+C65+D65</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3809,19 +3837,19 @@
       </c>
       <c r="B66" s="0" t="n">
         <f aca="false">B65-H$1*B65*C65</f>
-        <v>0.0990394470961825</v>
+        <v>0.101516806058505</v>
       </c>
       <c r="C66" s="0" t="n">
         <f aca="false">C65+H$1*B65*C65-F$1*C65</f>
-        <v>0.0128203498155258</v>
+        <v>0.0132780554615451</v>
       </c>
       <c r="D66" s="0" t="n">
         <f aca="false">D65+F$1*C65</f>
-        <v>0.898040203088292</v>
+        <v>0.88520513847995</v>
       </c>
       <c r="E66" s="0" t="n">
         <f aca="false">B66+C66+D66</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3830,19 +3858,19 @@
       </c>
       <c r="B67" s="0" t="n">
         <f aca="false">B66-H$1*B66*C66</f>
-        <v>0.0986162069770794</v>
+        <v>0.10106749079813</v>
       </c>
       <c r="C67" s="0" t="n">
         <f aca="false">C66+H$1*B66*C66-F$1*C66</f>
-        <v>0.0115342099592254</v>
+        <v>0.011956963327047</v>
       </c>
       <c r="D67" s="0" t="n">
         <f aca="false">D66+F$1*C66</f>
-        <v>0.899749583063695</v>
+        <v>0.886975545874823</v>
       </c>
       <c r="E67" s="0" t="n">
         <f aca="false">B67+C67+D67</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3851,19 +3879,19 @@
       </c>
       <c r="B68" s="0" t="n">
         <f aca="false">B67-H$1*B67*C67</f>
-        <v>0.0982370536315273</v>
+        <v>0.100664670704454</v>
       </c>
       <c r="C68" s="0" t="n">
         <f aca="false">C67+H$1*B67*C67-F$1*C67</f>
-        <v>0.0103754686435474</v>
+        <v>0.010765521643784</v>
       </c>
       <c r="D68" s="0" t="n">
         <f aca="false">D67+F$1*C67</f>
-        <v>0.901287477724925</v>
+        <v>0.888569807651762</v>
       </c>
       <c r="E68" s="0" t="n">
         <f aca="false">B68+C68+D68</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3872,19 +3900,19 @@
       </c>
       <c r="B69" s="0" t="n">
         <f aca="false">B68-H$1*B68*C68</f>
-        <v>0.0978973018083312</v>
+        <v>0.100303434807376</v>
       </c>
       <c r="C69" s="0" t="n">
         <f aca="false">C68+H$1*B68*C68-F$1*C68</f>
-        <v>0.00933182464760387</v>
+        <v>0.0096913546550239</v>
       </c>
       <c r="D69" s="0" t="n">
         <f aca="false">D68+F$1*C68</f>
-        <v>0.902670873544065</v>
+        <v>0.8900052105376</v>
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">B69+C69+D69</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3893,19 +3921,19 @@
       </c>
       <c r="B70" s="0" t="n">
         <f aca="false">B69-H$1*B69*C69</f>
-        <v>0.0975927816570149</v>
+        <v>0.0999794094207643</v>
       </c>
       <c r="C70" s="0" t="n">
         <f aca="false">C69+H$1*B69*C69-F$1*C69</f>
-        <v>0.00839210151257299</v>
+        <v>0.00872319942096583</v>
       </c>
       <c r="D70" s="0" t="n">
         <f aca="false">D69+F$1*C69</f>
-        <v>0.903915116830412</v>
+        <v>0.89129739115827</v>
       </c>
       <c r="E70" s="0" t="n">
         <f aca="false">B70+C70+D70</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3914,19 +3942,19 @@
       </c>
       <c r="B71" s="0" t="n">
         <f aca="false">B70-H$1*B70*C70</f>
-        <v>0.0973197788134949</v>
+        <v>0.0996886959786417</v>
       </c>
       <c r="C71" s="0" t="n">
         <f aca="false">C70+H$1*B70*C70-F$1*C70</f>
-        <v>0.00754615748774994</v>
+        <v>0.00785081960695963</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">D70+F$1*C70</f>
-        <v>0.905034063698755</v>
+        <v>0.892460484414399</v>
       </c>
       <c r="E71" s="0" t="n">
         <f aca="false">B71+C71+D71</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3935,19 +3963,19 @@
       </c>
       <c r="B72" s="0" t="n">
         <f aca="false">B71-H$1*B71*C71</f>
-        <v>0.0970749820209617</v>
+        <v>0.0994278166556479</v>
       </c>
       <c r="C72" s="0" t="n">
         <f aca="false">C71+H$1*B71*C71-F$1*C71</f>
-        <v>0.00678479994858315</v>
+        <v>0.0070649229823588</v>
       </c>
       <c r="D72" s="0" t="n">
         <f aca="false">D71+F$1*C71</f>
-        <v>0.906040218030455</v>
+        <v>0.893507260361993</v>
       </c>
       <c r="E72" s="0" t="n">
         <f aca="false">B72+C72+D72</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3956,19 +3984,19 @@
       </c>
       <c r="B73" s="0" t="n">
         <f aca="false">B72-H$1*B72*C72</f>
-        <v>0.0968554372432868</v>
+        <v>0.0991936666999892</v>
       </c>
       <c r="C73" s="0" t="n">
         <f aca="false">C72+H$1*B72*C72-F$1*C72</f>
-        <v>0.00609970473311358</v>
+        <v>0.00635708320703637</v>
       </c>
       <c r="D73" s="0" t="n">
         <f aca="false">D72+F$1*C72</f>
-        <v>0.906944858023599</v>
+        <v>0.894449250092975</v>
       </c>
       <c r="E73" s="0" t="n">
         <f aca="false">B73+C73+D73</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3977,19 +4005,19 @@
       </c>
       <c r="B74" s="0" t="n">
         <f aca="false">B73-H$1*B73*C73</f>
-        <v>0.09665850738696</v>
+        <v>0.0989834725690482</v>
       </c>
       <c r="C74" s="0" t="n">
         <f aca="false">C73+H$1*B73*C73-F$1*C73</f>
-        <v>0.00548334062502532</v>
+        <v>0.00571966624370581</v>
       </c>
       <c r="D74" s="0" t="n">
         <f aca="false">D73+F$1*C73</f>
-        <v>0.907758151988014</v>
+        <v>0.895296861187246</v>
       </c>
       <c r="E74" s="0" t="n">
         <f aca="false">B74+C74+D74</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3998,19 +4026,19 @@
       </c>
       <c r="B75" s="0" t="n">
         <f aca="false">B74-H$1*B74*C74</f>
-        <v>0.0964818368801902</v>
+        <v>0.0987947550934689</v>
       </c>
       <c r="C75" s="0" t="n">
         <f aca="false">C74+H$1*B74*C74-F$1*C74</f>
-        <v>0.00492889904845835</v>
+        <v>0.0051457615534577</v>
       </c>
       <c r="D75" s="0" t="n">
         <f aca="false">D74+F$1*C74</f>
-        <v>0.908489264071351</v>
+        <v>0.896059483353074</v>
       </c>
       <c r="E75" s="0" t="n">
         <f aca="false">B75+C75+D75</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4019,19 +4047,19 @@
       </c>
       <c r="B76" s="0" t="n">
         <f aca="false">B75-H$1*B75*C75</f>
-        <v>0.0963233204688595</v>
+        <v>0.0986252970093211</v>
       </c>
       <c r="C76" s="0" t="n">
         <f aca="false">C75+H$1*B75*C75-F$1*C75</f>
-        <v>0.00443022891999467</v>
+        <v>0.00462911809714442</v>
       </c>
       <c r="D76" s="0" t="n">
         <f aca="false">D75+F$1*C75</f>
-        <v>0.909146450611146</v>
+        <v>0.896745584893535</v>
       </c>
       <c r="E76" s="0" t="n">
         <f aca="false">B76+C76+D76</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4040,19 +4068,19 @@
       </c>
       <c r="B77" s="0" t="n">
         <f aca="false">B76-H$1*B76*C76</f>
-        <v>0.0961810756821891</v>
+        <v>0.0984731142935804</v>
       </c>
       <c r="C77" s="0" t="n">
         <f aca="false">C76+H$1*B76*C76-F$1*C76</f>
-        <v>0.0039817765173324</v>
+        <v>0.00416408506659919</v>
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">D76+F$1*C76</f>
-        <v>0.909737147800478</v>
+        <v>0.89736280063982</v>
       </c>
       <c r="E77" s="0" t="n">
         <f aca="false">B77+C77+D77</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4061,19 +4089,19 @@
       </c>
       <c r="B78" s="0" t="n">
         <f aca="false">B77-H$1*B77*C77</f>
-        <v>0.0960534184993347</v>
+        <v>0.0983364308186833</v>
       </c>
       <c r="C78" s="0" t="n">
         <f aca="false">C77+H$1*B77*C77-F$1*C77</f>
-        <v>0.00357853016454245</v>
+        <v>0.00374555719928311</v>
       </c>
       <c r="D78" s="0" t="n">
         <f aca="false">D77+F$1*C77</f>
-        <v>0.910268051336123</v>
+        <v>0.897918011982034</v>
       </c>
       <c r="E78" s="0" t="n">
         <f aca="false">B78+C78+D78</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4082,19 +4110,19 @@
       </c>
       <c r="B79" s="0" t="n">
         <f aca="false">B78-H$1*B78*C78</f>
-        <v>0.0959388418141656</v>
+        <v>0.0982136559098817</v>
       </c>
       <c r="C79" s="0" t="n">
         <f aca="false">C78+H$1*B78*C78-F$1*C78</f>
-        <v>0.00321596949443922</v>
+        <v>0.0033689244815136</v>
       </c>
       <c r="D79" s="0" t="n">
         <f aca="false">D78+F$1*C78</f>
-        <v>0.910745188691395</v>
+        <v>0.898417419608605</v>
       </c>
       <c r="E79" s="0" t="n">
         <f aca="false">B79+C79+D79</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4103,19 +4131,19 @@
       </c>
       <c r="B80" s="0" t="n">
         <f aca="false">B79-H$1*B79*C79</f>
-        <v>0.0958359963512969</v>
+        <v>0.0981033644466105</v>
       </c>
       <c r="C80" s="0" t="n">
         <f aca="false">C79+H$1*B79*C79-F$1*C79</f>
-        <v>0.00289001902471605</v>
+        <v>0.00303002601391637</v>
       </c>
       <c r="D80" s="0" t="n">
         <f aca="false">D79+F$1*C79</f>
-        <v>0.911173984623987</v>
+        <v>0.898866609539473</v>
       </c>
       <c r="E80" s="0" t="n">
         <f aca="false">B80+C80+D80</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4124,19 +4152,19 @@
       </c>
       <c r="B81" s="0" t="n">
         <f aca="false">B80-H$1*B80*C80</f>
-        <v>0.0957436737337276</v>
+        <v>0.0980042791978352</v>
       </c>
       <c r="C81" s="0" t="n">
         <f aca="false">C80+H$1*B80*C80-F$1*C80</f>
-        <v>0.0025970057723232</v>
+        <v>0.00272510779416951</v>
       </c>
       <c r="D81" s="0" t="n">
         <f aca="false">D80+F$1*C80</f>
-        <v>0.911559320493949</v>
+        <v>0.899270613007996</v>
       </c>
       <c r="E81" s="0" t="n">
         <f aca="false">B81+C81+D81</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4145,19 +4173,19 @@
       </c>
       <c r="B82" s="0" t="n">
         <f aca="false">B81-H$1*B81*C81</f>
-        <v>0.095660791442611</v>
+        <v>0.0979152551228005</v>
       </c>
       <c r="C82" s="0" t="n">
         <f aca="false">C81+H$1*B81*C81-F$1*C81</f>
-        <v>0.00233362062713008</v>
+        <v>0.0024507841633149</v>
       </c>
       <c r="D82" s="0" t="n">
         <f aca="false">D81+F$1*C81</f>
-        <v>0.911905587930259</v>
+        <v>0.899633960713885</v>
       </c>
       <c r="E82" s="0" t="n">
         <f aca="false">B82+C82+D82</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4166,19 +4194,19 @@
       </c>
       <c r="B83" s="0" t="n">
         <f aca="false">B82-H$1*B82*C82</f>
-        <v>0.095586379443905</v>
+        <v>0.0978352654039332</v>
       </c>
       <c r="C83" s="0" t="n">
         <f aca="false">C82+H$1*B82*C82-F$1*C82</f>
-        <v>0.00209688320888542</v>
+        <v>0.00220400266040688</v>
       </c>
       <c r="D83" s="0" t="n">
         <f aca="false">D82+F$1*C82</f>
-        <v>0.912216737347209</v>
+        <v>0.89996073193566</v>
       </c>
       <c r="E83" s="0" t="n">
         <f aca="false">B83+C83+D83</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4187,19 +4215,19 @@
       </c>
       <c r="B84" s="0" t="n">
         <f aca="false">B83-H$1*B83*C83</f>
-        <v>0.0955195682858869</v>
+        <v>0.0977633890088559</v>
       </c>
       <c r="C84" s="0" t="n">
         <f aca="false">C83+H$1*B83*C83-F$1*C83</f>
-        <v>0.00188410993905206</v>
+        <v>0.00198201203409659</v>
       </c>
       <c r="D84" s="0" t="n">
         <f aca="false">D83+F$1*C83</f>
-        <v>0.912496321775061</v>
+        <v>0.900254598957048</v>
       </c>
       <c r="E84" s="0" t="n">
         <f aca="false">B84+C84+D84</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4208,19 +4236,19 @@
       </c>
       <c r="B85" s="0" t="n">
         <f aca="false">B84-H$1*B84*C84</f>
-        <v>0.0954595784965598</v>
+        <v>0.0976987996043527</v>
       </c>
       <c r="C85" s="0" t="n">
         <f aca="false">C84+H$1*B84*C84-F$1*C84</f>
-        <v>0.00169288506983892</v>
+        <v>0.00178233316738692</v>
       </c>
       <c r="D85" s="0" t="n">
         <f aca="false">D84+F$1*C84</f>
-        <v>0.912747536433601</v>
+        <v>0.900518867228261</v>
       </c>
       <c r="E85" s="0" t="n">
         <f aca="false">B85+C85+D85</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4229,19 +4257,19 @@
       </c>
       <c r="B86" s="0" t="n">
         <f aca="false">B85-H$1*B85*C85</f>
-        <v>0.0954057111314898</v>
+        <v>0.0976407556673698</v>
       </c>
       <c r="C86" s="0" t="n">
         <f aca="false">C85+H$1*B85*C85-F$1*C85</f>
-        <v>0.00152103442559704</v>
+        <v>0.00160273268205157</v>
       </c>
       <c r="D86" s="0" t="n">
         <f aca="false">D85+F$1*C85</f>
-        <v>0.912973254442913</v>
+        <v>0.900756511650579</v>
       </c>
       <c r="E86" s="0" t="n">
         <f aca="false">B86+C86+D86</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4250,19 +4278,19 @@
       </c>
       <c r="B87" s="0" t="n">
         <f aca="false">B86-H$1*B86*C86</f>
-        <v>0.0953573393411466</v>
+        <v>0.0975885916573004</v>
       </c>
       <c r="C87" s="0" t="n">
         <f aca="false">C86+H$1*B86*C86-F$1*C86</f>
-        <v>0.00136660162586062</v>
+        <v>0.0014411990011808</v>
       </c>
       <c r="D87" s="0" t="n">
         <f aca="false">D86+F$1*C86</f>
-        <v>0.913176059032992</v>
+        <v>0.900970209341519</v>
       </c>
       <c r="E87" s="0" t="n">
         <f aca="false">B87+C87+D87</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4271,19 +4299,19 @@
       </c>
       <c r="B88" s="0" t="n">
         <f aca="false">B87-H$1*B87*C87</f>
-        <v>0.0953139008428195</v>
+        <v>0.0975417101303593</v>
       </c>
       <c r="C88" s="0" t="n">
         <f aca="false">C87+H$1*B87*C87-F$1*C87</f>
-        <v>0.00122782657407299</v>
+        <v>0.00129592066129774</v>
       </c>
       <c r="D88" s="0" t="n">
         <f aca="false">D87+F$1*C87</f>
-        <v>0.913358272583107</v>
+        <v>0.901162369208343</v>
       </c>
       <c r="E88" s="0" t="n">
         <f aca="false">B88+C88+D88</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4292,19 +4320,19 @@
       </c>
       <c r="B89" s="0" t="n">
         <f aca="false">B88-H$1*B88*C88</f>
-        <v>0.0952748911960417</v>
+        <v>0.0974995746911939</v>
       </c>
       <c r="C89" s="0" t="n">
         <f aca="false">C88+H$1*B88*C88-F$1*C88</f>
-        <v>0.00110312601097438</v>
+        <v>0.00116526667895679</v>
       </c>
       <c r="D89" s="0" t="n">
         <f aca="false">D88+F$1*C88</f>
-        <v>0.913521982792984</v>
+        <v>0.901335158629849</v>
       </c>
       <c r="E89" s="0" t="n">
         <f aca="false">B89+C89+D89</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4313,19 +4341,19 @@
       </c>
       <c r="B90" s="0" t="n">
         <f aca="false">B89-H$1*B89*C89</f>
-        <v>0.0952398577924847</v>
+        <v>0.0974617036893272</v>
       </c>
       <c r="C90" s="0" t="n">
         <f aca="false">C89+H$1*B89*C89-F$1*C89</f>
-        <v>0.000991075946401502</v>
+        <v>0.00104776879029592</v>
       </c>
       <c r="D90" s="0" t="n">
         <f aca="false">D89+F$1*C89</f>
-        <v>0.913669066261114</v>
+        <v>0.901490527520377</v>
       </c>
       <c r="E90" s="0" t="n">
         <f aca="false">B90+C90+D90</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4334,19 +4362,19 @@
       </c>
       <c r="B91" s="0" t="n">
         <f aca="false">B90-H$1*B90*C90</f>
-        <v>0.0952083944817524</v>
+        <v>0.0974276645788689</v>
       </c>
       <c r="C91" s="0" t="n">
         <f aca="false">C90+H$1*B90*C90-F$1*C90</f>
-        <v>0.000890395797613579</v>
+        <v>0.000942105395381382</v>
       </c>
       <c r="D91" s="0" t="n">
         <f aca="false">D90+F$1*C90</f>
-        <v>0.913801209720634</v>
+        <v>0.90163023002575</v>
       </c>
       <c r="E91" s="0" t="n">
         <f aca="false">B91+C91+D91</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4355,19 +4383,19 @@
       </c>
       <c r="B92" s="0" t="n">
         <f aca="false">B91-H$1*B91*C91</f>
-        <v>0.0951801367636377</v>
+        <v>0.0973970688693826</v>
       </c>
       <c r="C92" s="0" t="n">
         <f aca="false">C91+H$1*B91*C91-F$1*C91</f>
-        <v>0.000799934076046465</v>
+        <v>0.000847087052150251</v>
       </c>
       <c r="D92" s="0" t="n">
         <f aca="false">D91+F$1*C91</f>
-        <v>0.913919929160315</v>
+        <v>0.901755844078467</v>
       </c>
       <c r="E92" s="0" t="n">
         <f aca="false">B92+C92+D92</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4376,19 +4404,19 @@
       </c>
       <c r="B93" s="0" t="n">
         <f aca="false">B92-H$1*B92*C92</f>
-        <v>0.0951547574853844</v>
+        <v>0.0973695676040637</v>
       </c>
       <c r="C93" s="0" t="n">
         <f aca="false">C92+H$1*B92*C92-F$1*C92</f>
-        <v>0.000718655477493602</v>
+        <v>0.000761643377182432</v>
       </c>
       <c r="D93" s="0" t="n">
         <f aca="false">D92+F$1*C92</f>
-        <v>0.914026587037122</v>
+        <v>0.901868789018754</v>
       </c>
       <c r="E93" s="0" t="n">
         <f aca="false">B93+C93+D93</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4397,19 +4425,19 @@
       </c>
       <c r="B94" s="0" t="n">
         <f aca="false">B93-H$1*B93*C93</f>
-        <v>0.0951319629894922</v>
+        <v>0.0973448473086288</v>
       </c>
       <c r="C94" s="0" t="n">
         <f aca="false">C93+H$1*B93*C93-F$1*C93</f>
-        <v>0.00064562924305327</v>
+        <v>0.000684811222326358</v>
       </c>
       <c r="D94" s="0" t="n">
         <f aca="false">D93+F$1*C93</f>
-        <v>0.914122407767454</v>
+        <v>0.901970341469045</v>
       </c>
       <c r="E94" s="0" t="n">
         <f aca="false">B94+C94+D94</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4418,19 +4446,19 @@
       </c>
       <c r="B95" s="0" t="n">
         <f aca="false">B94-H$1*B94*C94</f>
-        <v>0.0951114896637405</v>
+        <v>0.0973226263606712</v>
       </c>
       <c r="C95" s="0" t="n">
         <f aca="false">C94+H$1*B94*C94-F$1*C94</f>
-        <v>0.000580018669731194</v>
+        <v>0.000615724007307042</v>
       </c>
       <c r="D95" s="0" t="n">
         <f aca="false">D94+F$1*C94</f>
-        <v>0.914208491666528</v>
+        <v>0.902061649632022</v>
       </c>
       <c r="E95" s="0" t="n">
         <f aca="false">B95+C95+D95</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4439,19 +4467,19 @@
       </c>
       <c r="B96" s="0" t="n">
         <f aca="false">B95-H$1*B95*C95</f>
-        <v>0.0950931008505035</v>
+        <v>0.0973026517348364</v>
       </c>
       <c r="C96" s="0" t="n">
         <f aca="false">C95+H$1*B95*C95-F$1*C95</f>
-        <v>0.000521071660337339</v>
+        <v>0.00055360209883425</v>
       </c>
       <c r="D96" s="0" t="n">
         <f aca="false">D95+F$1*C95</f>
-        <v>0.914285827489159</v>
+        <v>0.902143746166329</v>
       </c>
       <c r="E96" s="0" t="n">
         <f aca="false">B96+C96+D96</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4460,19 +4488,19 @@
       </c>
       <c r="B97" s="0" t="n">
         <f aca="false">B96-H$1*B96*C96</f>
-        <v>0.095076584077188</v>
+        <v>0.0972846960840956</v>
       </c>
       <c r="C97" s="0" t="n">
         <f aca="false">C96+H$1*B96*C96-F$1*C96</f>
-        <v>0.000468112212274627</v>
+        <v>0.000497744136397198</v>
       </c>
       <c r="D97" s="0" t="n">
         <f aca="false">D96+F$1*C96</f>
-        <v>0.914355303710537</v>
+        <v>0.902217559779507</v>
       </c>
       <c r="E97" s="0" t="n">
         <f aca="false">B97+C97+D97</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4481,19 +4509,19 @@
       </c>
       <c r="B98" s="0" t="n">
         <f aca="false">B97-H$1*B97*C97</f>
-        <v>0.0950617485738187</v>
+        <v>0.0972685551217499</v>
       </c>
       <c r="C98" s="0" t="n">
         <f aca="false">C97+H$1*B97*C97-F$1*C97</f>
-        <v>0.000420532754007306</v>
+        <v>0.000447519213889919</v>
       </c>
       <c r="D98" s="0" t="n">
         <f aca="false">D97+F$1*C97</f>
-        <v>0.914417718672174</v>
+        <v>0.90228392566436</v>
       </c>
       <c r="E98" s="0" t="n">
         <f aca="false">B98+C98+D98</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4502,19 +4530,19 @@
       </c>
       <c r="B99" s="0" t="n">
         <f aca="false">B98-H$1*B98*C98</f>
-        <v>0.0950484230475091</v>
+        <v>0.0972540452726418</v>
       </c>
       <c r="C99" s="0" t="n">
         <f aca="false">C98+H$1*B98*C98-F$1*C98</f>
-        <v>0.000377787246449164</v>
+        <v>0.000402359834479361</v>
       </c>
       <c r="D99" s="0" t="n">
         <f aca="false">D98+F$1*C98</f>
-        <v>0.914473789706041</v>
+        <v>0.902343594892879</v>
       </c>
       <c r="E99" s="0" t="n">
         <f aca="false">B99+C99+D99</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4523,19 +4551,19 @@
       </c>
       <c r="B100" s="0" t="n">
         <f aca="false">B99-H$1*B99*C99</f>
-        <v>0.095036453686835</v>
+        <v>0.0972410015654557</v>
       </c>
       <c r="C100" s="0" t="n">
         <f aca="false">C99+H$1*B99*C99-F$1*C99</f>
-        <v>0.000339384974263427</v>
+        <v>0.000361755563734896</v>
       </c>
       <c r="D100" s="0" t="n">
         <f aca="false">D99+F$1*C99</f>
-        <v>0.914524161338901</v>
+        <v>0.90239724287081</v>
       </c>
       <c r="E100" s="0" t="n">
         <f aca="false">B100+C100+D100</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4544,19 +4572,19 @@
       </c>
       <c r="B101" s="0" t="n">
         <f aca="false">B100-H$1*B100*C100</f>
-        <v>0.0950257023720388</v>
+        <v>0.0972292757410092</v>
       </c>
       <c r="C101" s="0" t="n">
         <f aca="false">C100+H$1*B100*C100-F$1*C100</f>
-        <v>0.000304884959157835</v>
+        <v>0.000325247313016729</v>
       </c>
       <c r="D101" s="0" t="n">
         <f aca="false">D100+F$1*C100</f>
-        <v>0.914569412668803</v>
+        <v>0.902445476945974</v>
       </c>
       <c r="E101" s="0" t="n">
         <f aca="false">B101+C101+D101</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4565,19 +4593,19 @@
       </c>
       <c r="B102" s="0" t="n">
         <f aca="false">B101-H$1*B101*C101</f>
-        <v>0.0950160450695766</v>
+        <v>0.0972187345541154</v>
       </c>
       <c r="C102" s="0" t="n">
         <f aca="false">C101+H$1*B101*C101-F$1*C101</f>
-        <v>0.000273890933732338</v>
+        <v>0.000292422191508274</v>
       </c>
       <c r="D102" s="0" t="n">
         <f aca="false">D101+F$1*C101</f>
-        <v>0.914610063996691</v>
+        <v>0.902488843254376</v>
       </c>
       <c r="E102" s="0" t="n">
         <f aca="false">B102+C102+D102</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4586,19 +4614,19 @@
       </c>
       <c r="B103" s="0" t="n">
         <f aca="false">B102-H$1*B102*C102</f>
-        <v>0.0950073703918087</v>
+        <v>0.0972092582489774</v>
       </c>
       <c r="C103" s="0" t="n">
         <f aca="false">C102+H$1*B102*C102-F$1*C102</f>
-        <v>0.000246046820335913</v>
+        <v>0.000262908871111829</v>
       </c>
       <c r="D103" s="0" t="n">
         <f aca="false">D102+F$1*C102</f>
-        <v>0.914646582787855</v>
+        <v>0.902527832879911</v>
       </c>
       <c r="E103" s="0" t="n">
         <f aca="false">B103+C103+D103</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4607,19 +4635,19 @@
       </c>
       <c r="B104" s="0" t="n">
         <f aca="false">B103-H$1*B103*C103</f>
-        <v>0.0949995783046776</v>
+        <v>0.0972007391901948</v>
       </c>
       <c r="C104" s="0" t="n">
         <f aca="false">C103+H$1*B103*C103-F$1*C103</f>
-        <v>0.000221032664755585</v>
+        <v>0.000236373413746205</v>
       </c>
       <c r="D104" s="0" t="n">
         <f aca="false">D103+F$1*C103</f>
-        <v>0.914679389030566</v>
+        <v>0.902562887396059</v>
       </c>
       <c r="E104" s="0" t="n">
         <f aca="false">B104+C104+D104</f>
-        <v>1.0099</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>